<commit_message>
Done the author's import
</commit_message>
<xml_diff>
--- a/teg_asovac_src/upload/cargaAutores.xlsx
+++ b/teg_asovac_src/upload/cargaAutores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">Nombres(*)</t>
   </si>
@@ -88,10 +88,19 @@
     <t xml:space="preserve">o@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">pruebad</t>
+  </si>
+  <si>
     <t xml:space="preserve">S</t>
   </si>
   <si>
+    <t xml:space="preserve">caracas</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bachiller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ninguna</t>
   </si>
   <si>
     <t xml:space="preserve">computacion</t>
@@ -213,24 +222,23 @@
   </sheetPr>
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.9336734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -308,26 +316,35 @@
       <c r="G2" s="0" t="n">
         <v>25454546675</v>
       </c>
+      <c r="H2" s="0" t="s">
+        <v>22</v>
+      </c>
       <c r="I2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>24</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>26</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now when some user import authors by excel, the authors created receive a mail with his user and his password
</commit_message>
<xml_diff>
--- a/teg_asovac_src/upload/cargaAutores.xlsx
+++ b/teg_asovac_src/upload/cargaAutores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t xml:space="preserve">Nombres(*)</t>
   </si>
@@ -116,6 +116,45 @@
   </si>
   <si>
     <t xml:space="preserve">UCV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prueba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">final</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V585</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guarenas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Licenciado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">humanidades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">derecho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">universidad de prueba</t>
   </si>
 </sst>
 </file>
@@ -125,7 +164,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -146,6 +185,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -190,7 +236,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -201,6 +247,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -220,10 +270,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -347,7 +397,57 @@
         <v>31</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>54454545455</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>45454545455</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" display="a@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
NOw create the arbitro's instance when create/import authors
</commit_message>
<xml_diff>
--- a/teg_asovac_src/upload/cargaAutores.xlsx
+++ b/teg_asovac_src/upload/cargaAutores.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t xml:space="preserve">Nombres(*)</t>
   </si>
@@ -73,6 +73,51 @@
     <t xml:space="preserve">Universidad(*)</t>
   </si>
   <si>
+    <t xml:space="preserve">Línea de investigación(*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prueba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">final</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V585</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guarenas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Licenciado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">humanidades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">derecho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">universidad de prueba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
     <t xml:space="preserve">Osvani Enrique</t>
   </si>
   <si>
@@ -116,45 +161,6 @@
   </si>
   <si>
     <t xml:space="preserve">UCV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prueba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">final</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V585</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guarenas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Licenciado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ok</t>
-  </si>
-  <si>
-    <t xml:space="preserve">humanidades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">derecho</t>
-  </si>
-  <si>
-    <t xml:space="preserve">universidad de prueba</t>
   </si>
 </sst>
 </file>
@@ -164,7 +170,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -185,6 +191,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -236,21 +249,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -270,25 +287,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:Q4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S:S"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.9336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="19.2142857142857"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.2857142857143"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -343,57 +368,57 @@
       <c r="Q1" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="C2" s="0" t="s">
+        <v>20</v>
+      </c>
       <c r="D2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>32323244244</v>
+        <v>54454545455</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>25454546675</v>
+        <v>45454545455</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="Q2" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="R2" s="0" t="s">
         <v>31</v>
       </c>
     </row>
@@ -404,20 +429,20 @@
       <c r="B3" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>54454545455</v>
+      <c r="F3" s="3" t="n">
+        <v>45454545454</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>45454545455</v>
+        <v>25454546675</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>37</v>
@@ -440,13 +465,22 @@
       <c r="N3" s="0" t="s">
         <v>43</v>
       </c>
+      <c r="O3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="Q3" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="a@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId1" display="a@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Now the import generate only 1 message to show in a future file that will be downloaded
</commit_message>
<xml_diff>
--- a/teg_asovac_src/upload/cargaAutores.xlsx
+++ b/teg_asovac_src/upload/cargaAutores.xlsx
@@ -287,10 +287,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S:S"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -423,58 +423,61 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B4" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F4" s="3" t="n">
         <v>45454545454</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G4" s="0" t="n">
         <v>25454546675</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H4" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I4" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J4" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K4" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="L4" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M4" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="N4" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="O4" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="P4" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="Q4" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="R3" s="0" t="s">
+      <c r="R4" s="0" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deleted the linea investigacion's field from authors, the arbitro's instance dont need it for his creation
</commit_message>
<xml_diff>
--- a/teg_asovac_src/upload/cargaAutores.xlsx
+++ b/teg_asovac_src/upload/cargaAutores.xlsx
@@ -200,6 +200,7 @@
       <charset val="1"/>
     </font>
     <font>
+      <u val="single"/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
@@ -287,10 +288,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -372,112 +373,109 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>54454545455</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>45454545455</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="N2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="Q2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="R2" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F3" s="3" t="n">
         <v>45454545454</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G3" s="0" t="n">
         <v>25454546675</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="K3" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="0" t="s">
+      <c r="L3" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="M3" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="0" t="s">
+      <c r="N3" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="O4" s="0" t="s">
+      <c r="O3" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="P4" s="0" t="s">
+      <c r="P3" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="Q3" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="R4" s="0" t="s">
+      <c r="R3" s="0" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Now when an error occur an error log will be downloaded
</commit_message>
<xml_diff>
--- a/teg_asovac_src/upload/cargaAutores.xlsx
+++ b/teg_asovac_src/upload/cargaAutores.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t xml:space="preserve">Nombres(*)</t>
   </si>
@@ -73,9 +73,6 @@
     <t xml:space="preserve">Universidad(*)</t>
   </si>
   <si>
-    <t xml:space="preserve">Línea de investigación(*)</t>
-  </si>
-  <si>
     <t xml:space="preserve">prueba</t>
   </si>
   <si>
@@ -106,18 +103,15 @@
     <t xml:space="preserve">Ok</t>
   </si>
   <si>
-    <t xml:space="preserve">humanidades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">derecho</t>
+    <t xml:space="preserve">Ciencias Sociales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ciencias sociales</t>
   </si>
   <si>
     <t xml:space="preserve">universidad de prueba</t>
   </si>
   <si>
-    <t xml:space="preserve">X</t>
-  </si>
-  <si>
     <t xml:space="preserve">Osvani Enrique</t>
   </si>
   <si>
@@ -148,16 +142,13 @@
     <t xml:space="preserve">ninguna</t>
   </si>
   <si>
-    <t xml:space="preserve">computacion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">desarrollo web</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cuantica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">robotica</t>
+    <t xml:space="preserve">biociencias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medicina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">farmacologia</t>
   </si>
   <si>
     <t xml:space="preserve">UCV</t>
@@ -288,33 +279,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="19.2142857142857"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.2857142857143"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="19.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -369,25 +360,22 @@
       <c r="Q1" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>54454545455</v>
@@ -396,48 +384,45 @@
         <v>45454545455</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>45454545454</v>
@@ -446,37 +431,31 @@
         <v>25454546675</v>
       </c>
       <c r="H3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="K3" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="L3" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="M3" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="N3" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="O3" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="Q3" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="P3" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q3" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="R3" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -485,10 +464,10 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed error when use the área/subarea/universidad name have special characters in authors import
</commit_message>
<xml_diff>
--- a/teg_asovac_src/upload/cargaAutores.xlsx
+++ b/teg_asovac_src/upload/cargaAutores.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t xml:space="preserve">Nombres(*)</t>
   </si>
@@ -103,52 +103,49 @@
     <t xml:space="preserve">Ok</t>
   </si>
   <si>
-    <t xml:space="preserve">Ciencias Sociales</t>
+    <t xml:space="preserve">congreso de la sociedad venezolana de física</t>
+  </si>
+  <si>
+    <t xml:space="preserve">física nuclear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">universidad de prueba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Osvani Enrique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colina Jimenez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V584</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pruebad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">caracas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bachiller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ninguna</t>
   </si>
   <si>
     <t xml:space="preserve">ciencias sociales</t>
   </si>
   <si>
-    <t xml:space="preserve">universidad de prueba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Osvani Enrique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Colina Jimenez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V584</t>
-  </si>
-  <si>
-    <t xml:space="preserve">o@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pruebad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">caracas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bachiller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ninguna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biociencias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">medicina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">farmacologia</t>
+    <t xml:space="preserve">educación</t>
   </si>
   <si>
     <t xml:space="preserve">UCV</t>
@@ -279,33 +276,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1:R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="19.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="20.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.37"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -360,6 +356,7 @@
       <c r="Q1" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="S1" s="0"/>
     </row>
     <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -452,10 +449,10 @@
         <v>41</v>
       </c>
       <c r="O3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q3" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="Q3" s="0" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -464,10 +461,10 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>